<commit_message>
Fixes and new Script
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C120CFA4-5640-418A-9277-CCD676C2C156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{ED38C219-2071-4222-BC2F-5DBB436AA0F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -13,10 +13,14 @@
     <sheet name="verifyTheProductLink" sheetId="7" r:id="rId3"/>
     <sheet name="clickOnOuLink" sheetId="5" r:id="rId4"/>
     <sheet name="verifyTheSearch" sheetId="6" r:id="rId5"/>
-    <sheet name="CreateAccountTest" sheetId="4" r:id="rId6"/>
+    <sheet name="verifyTheSearchFullname" sheetId="9" r:id="rId6"/>
+    <sheet name="verifyTheSearchOneAlphabet" sheetId="10" r:id="rId7"/>
+    <sheet name="verifyTheValidationmessage" sheetId="11" r:id="rId8"/>
+    <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId9"/>
+    <sheet name="CreateAccountTest" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L7"/>
+  <oleSize ref="A1:R17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Raman</t>
   </si>
@@ -64,9 +68,6 @@
     <t>Hyde@2317</t>
   </si>
   <si>
-    <t>SearchItem</t>
-  </si>
-  <si>
     <t>Guy Markers</t>
   </si>
   <si>
@@ -74,6 +75,12 @@
   </si>
   <si>
     <t>Pole Restoration</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>"    "</t>
   </si>
 </sst>
 </file>
@@ -443,6 +450,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
@@ -582,9 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E0D8D1-9273-4970-9251-8B99B2980E37}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -596,50 +629,84 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF90B1B-57B5-4414-AC3B-569DC6A7BEA8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05950B89-E92A-4646-9694-E3FEC191FBC5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10C5F3C-EFE8-4B4F-A0A0-153F52BCD7A9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" activeCellId="1" sqref="A1 C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468D2C47-00AC-4DF8-AF6F-D0EF06E8D38F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit 2 September 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4FDF7D68-4A23-4D54-990D-A3C61DE57FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB20EB87-C8E7-4780-A522-DF837644B312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20790" windowHeight="11820" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -19,9 +24,13 @@
     <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId9"/>
     <sheet name="CreateAccountTest" sheetId="4" r:id="rId10"/>
     <sheet name="verifyTheSearchCrossButton" sheetId="12" r:id="rId11"/>
+    <sheet name="verifyDynamicDropdown" sheetId="13" r:id="rId12"/>
+    <sheet name="verifySearchResultsOnTyping" sheetId="14" r:id="rId13"/>
+    <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId14"/>
+    <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId15"/>
+    <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Raman</t>
   </si>
@@ -85,6 +94,36 @@
   </si>
   <si>
     <t xml:space="preserve">               </t>
+  </si>
+  <si>
+    <t>AskOsmoseSearch</t>
+  </si>
+  <si>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>TypeJointUse</t>
+  </si>
+  <si>
+    <t>Joint Use</t>
+  </si>
+  <si>
+    <t>TypeJointUseInSearchbox</t>
+  </si>
+  <si>
+    <t>NoResults</t>
+  </si>
+  <si>
+    <t>Noresultsfound</t>
+  </si>
+  <si>
+    <t>TypeJointUseTextUpdation</t>
+  </si>
+  <si>
+    <t>TypePoleReplacementTextUpdation</t>
+  </si>
+  <si>
+    <t>Pole Replacement</t>
   </si>
 </sst>
 </file>
@@ -486,20 +525,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2D0FF7-8259-4C88-ABF2-E9337205FC0D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DA5B9-7278-497C-93B8-35FED90EB872}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62C1E2F-C94F-40C3-A706-17602DE60785}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21843DF4-A28F-40DD-9ED6-86F66E6C735F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2497EB80-35A2-4AAD-9C1D-AEDB0EC50212}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B1B0C-F841-42B8-A0C1-21DBCE8A2DC8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +814,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E0D8D1-9273-4970-9251-8B99B2980E37}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -654,18 +824,16 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit 21 September 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB20EB87-C8E7-4780-A522-DF837644B312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5069C-A044-474D-8AAE-B63F49F416ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,11 @@
     <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId14"/>
     <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId15"/>
     <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId16"/>
+    <sheet name="verifySearchWebinarsHistorical" sheetId="18" r:id="rId17"/>
+    <sheet name="verifyInvalidSearchHistorical" sheetId="19" r:id="rId18"/>
+    <sheet name="verifySortWebinarsHistorical" sheetId="20" r:id="rId19"/>
+    <sheet name="verifyClearSearchHistorical" sheetId="21" r:id="rId20"/>
+    <sheet name="verifyExternalVideo" sheetId="22" r:id="rId21"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Raman</t>
   </si>
@@ -124,6 +129,27 @@
   </si>
   <si>
     <t>Pole Replacement</t>
+  </si>
+  <si>
+    <t>TypeHistoricalSearchBar</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>TypeHistoricalSearchBarInvalid</t>
+  </si>
+  <si>
+    <t>AutomatedTesting</t>
+  </si>
+  <si>
+    <t>TypeHistoricalSearchBarSort</t>
+  </si>
+  <si>
+    <t>TypeHistoricalClearSearch</t>
+  </si>
+  <si>
+    <t>TypeExternal</t>
   </si>
 </sst>
 </file>
@@ -650,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B1B0C-F841-42B8-A0C1-21DBCE8A2DC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -670,6 +696,87 @@
       </c>
       <c r="B2" t="s">
         <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C461882E-5B05-4789-AF09-7737EACBFC43}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B5B726-6BA8-4E09-89C1-3903738DA995}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C27DB-E6DA-4A1F-9493-A165D018979A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -722,6 +829,57 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE935E1F-C13E-4D89-A48B-2CD047CED7EB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D1169F-C9EA-4258-B52F-834B03470238}">
   <dimension ref="A1:C2"/>

</xml_diff>

<commit_message>
Commit 1 October 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\Osmose360Dev\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5069C-A044-474D-8AAE-B63F49F416ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37A46B8-D09F-47CB-9C5B-FB92B49C134A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Raman</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>TypeExternal</t>
+  </si>
+  <si>
+    <t>varun.magadiranganath@centurylink.com</t>
+  </si>
+  <si>
+    <t>Qwerty1@</t>
   </si>
 </sst>
 </file>
@@ -788,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +817,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -822,8 +828,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{07147E0C-2C00-49B1-AB63-BC0F9B4B4701}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -861,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Commit 12 Oct 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\Osmose360Test\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5069C-A044-474D-8AAE-B63F49F416ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECA5880-692A-4BE7-96F0-C44842AD8BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Raman</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>TypeExternal</t>
+  </si>
+  <si>
+    <t>Qwerty1@</t>
+  </si>
+  <si>
+    <t>varun.magadiranganath@centurylink.com</t>
   </si>
 </sst>
 </file>
@@ -788,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +817,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -861,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Commit 20 october 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE5069C-A044-474D-8AAE-B63F49F416ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3162845-91D2-4348-852F-AC31E1AE0D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -104,12 +104,6 @@
     <t>AskOsmoseSearch</t>
   </si>
   <si>
-    <t>Ind</t>
-  </si>
-  <si>
-    <t>TypeJointUse</t>
-  </si>
-  <si>
     <t>Joint Use</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>TypeExternal</t>
+  </si>
+  <si>
+    <t>TypePoleReplacement</t>
+  </si>
+  <si>
+    <t>Indus</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DA5B9-7278-497C-93B8-35FED90EB872}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -589,7 +589,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -602,19 +602,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -634,12 +634,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -659,12 +659,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -684,18 +684,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -718,12 +718,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -743,12 +743,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -771,12 +771,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -844,12 +844,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -861,18 +861,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit 17 November 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -1,39 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3162845-91D2-4348-852F-AC31E1AE0D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F165C2-7B34-460D-8672-6DA7AEDFA4DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="loginTest" sheetId="1" r:id="rId2"/>
-    <sheet name="verifyTheProductLink" sheetId="7" r:id="rId3"/>
-    <sheet name="clickOnOuLink" sheetId="5" r:id="rId4"/>
-    <sheet name="verifyTheSearch" sheetId="6" r:id="rId5"/>
-    <sheet name="verifyTheSearchFullname" sheetId="9" r:id="rId6"/>
-    <sheet name="verifyTheSearchOneAlphabet" sheetId="10" r:id="rId7"/>
-    <sheet name="verifyTheValidationmessage" sheetId="11" r:id="rId8"/>
-    <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId9"/>
-    <sheet name="CreateAccountTest" sheetId="4" r:id="rId10"/>
-    <sheet name="verifyTheSearchCrossButton" sheetId="12" r:id="rId11"/>
-    <sheet name="verifyDynamicDropdown" sheetId="13" r:id="rId12"/>
-    <sheet name="verifySearchResultsOnTyping" sheetId="14" r:id="rId13"/>
-    <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId14"/>
-    <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId15"/>
-    <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId16"/>
-    <sheet name="verifySearchWebinarsHistorical" sheetId="18" r:id="rId17"/>
-    <sheet name="verifyInvalidSearchHistorical" sheetId="19" r:id="rId18"/>
-    <sheet name="verifySortWebinarsHistorical" sheetId="20" r:id="rId19"/>
-    <sheet name="verifyClearSearchHistorical" sheetId="21" r:id="rId20"/>
-    <sheet name="verifyExternalVideo" sheetId="22" r:id="rId21"/>
+    <sheet name="ocalcloginTestNormal" sheetId="23" r:id="rId3"/>
+    <sheet name="ocalcloginTestAdmin" sheetId="24" r:id="rId4"/>
+    <sheet name="verifyTheProductLink" sheetId="7" r:id="rId5"/>
+    <sheet name="clickOnOuLink" sheetId="5" r:id="rId6"/>
+    <sheet name="verifyTheSearch" sheetId="6" r:id="rId7"/>
+    <sheet name="verifyTheSearchFullname" sheetId="9" r:id="rId8"/>
+    <sheet name="verifyTheSearchOneAlphabet" sheetId="10" r:id="rId9"/>
+    <sheet name="verifyTheValidationmessage" sheetId="11" r:id="rId10"/>
+    <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId11"/>
+    <sheet name="CreateAccountTest" sheetId="4" r:id="rId12"/>
+    <sheet name="verifyTheSearchCrossButton" sheetId="12" r:id="rId13"/>
+    <sheet name="verifyDynamicDropdown" sheetId="13" r:id="rId14"/>
+    <sheet name="verifySearchResultsOnTyping" sheetId="14" r:id="rId15"/>
+    <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId16"/>
+    <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId17"/>
+    <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId18"/>
+    <sheet name="verifySearchWebinarsHistorical" sheetId="18" r:id="rId19"/>
+    <sheet name="verifyInvalidSearchHistorical" sheetId="19" r:id="rId20"/>
+    <sheet name="verifySortWebinarsHistorical" sheetId="20" r:id="rId21"/>
+    <sheet name="verifyClearSearchHistorical" sheetId="21" r:id="rId22"/>
+    <sheet name="verifyExternalVideo" sheetId="22" r:id="rId23"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Raman</t>
   </si>
@@ -150,6 +152,18 @@
   </si>
   <si>
     <t>Indus</t>
+  </si>
+  <si>
+    <t>shanthling.kodli@centurylink.com</t>
+  </si>
+  <si>
+    <t>Denver*235</t>
+  </si>
+  <si>
+    <t>prime@12345</t>
+  </si>
+  <si>
+    <t>mohammedjunaid.kaikade@centurylink.com</t>
   </si>
 </sst>
 </file>
@@ -520,6 +534,57 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10C5F3C-EFE8-4B4F-A0A0-153F52BCD7A9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468D2C47-00AC-4DF8-AF6F-D0EF06E8D38F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -547,7 +612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2D0FF7-8259-4C88-ABF2-E9337205FC0D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -572,11 +637,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DA5B9-7278-497C-93B8-35FED90EB872}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -597,7 +662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62C1E2F-C94F-40C3-A706-17602DE60785}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -622,7 +687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21843DF4-A28F-40DD-9ED6-86F66E6C735F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -647,7 +712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2497EB80-35A2-4AAD-9C1D-AEDB0EC50212}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -672,7 +737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B1B0C-F841-42B8-A0C1-21DBCE8A2DC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -703,7 +768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C461882E-5B05-4789-AF09-7737EACBFC43}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -719,59 +784,6 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B5B726-6BA8-4E09-89C1-3903738DA995}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C27DB-E6DA-4A1F-9493-A165D018979A}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -789,7 +801,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,6 +842,59 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B5B726-6BA8-4E09-89C1-3903738DA995}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C27DB-E6DA-4A1F-9493-A165D018979A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE935E1F-C13E-4D89-A48B-2CD047CED7EB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -857,7 +922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -881,6 +946,76 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157B7B6B-70F3-4A49-967B-A759A4B063A2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDD2788-B65D-460D-8E6B-4273352A50D8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D1169F-C9EA-4258-B52F-834B03470238}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -925,7 +1060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD1348E-0969-4054-A1EA-4AAF0CCB32EA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -970,7 +1105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E0D8D1-9273-4970-9251-8B99B2980E37}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -998,7 +1133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF90B1B-57B5-4414-AC3B-569DC6A7BEA8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1024,7 +1159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05950B89-E92A-4646-9694-E3FEC191FBC5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1045,55 +1180,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10C5F3C-EFE8-4B4F-A0A0-153F52BCD7A9}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468D2C47-00AC-4DF8-AF6F-D0EF06E8D38F}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 26 Nov 20
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -8,34 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F165C2-7B34-460D-8672-6DA7AEDFA4DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EFCEE2-8DFB-4D80-9BE2-1749E1231699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="loginTest" sheetId="1" r:id="rId2"/>
     <sheet name="ocalcloginTestNormal" sheetId="23" r:id="rId3"/>
     <sheet name="ocalcloginTestAdmin" sheetId="24" r:id="rId4"/>
-    <sheet name="verifyTheProductLink" sheetId="7" r:id="rId5"/>
-    <sheet name="clickOnOuLink" sheetId="5" r:id="rId6"/>
-    <sheet name="verifyTheSearch" sheetId="6" r:id="rId7"/>
-    <sheet name="verifyTheSearchFullname" sheetId="9" r:id="rId8"/>
-    <sheet name="verifyTheSearchOneAlphabet" sheetId="10" r:id="rId9"/>
-    <sheet name="verifyTheValidationmessage" sheetId="11" r:id="rId10"/>
-    <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId11"/>
-    <sheet name="CreateAccountTest" sheetId="4" r:id="rId12"/>
-    <sheet name="verifyTheSearchCrossButton" sheetId="12" r:id="rId13"/>
-    <sheet name="verifyDynamicDropdown" sheetId="13" r:id="rId14"/>
-    <sheet name="verifySearchResultsOnTyping" sheetId="14" r:id="rId15"/>
-    <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId16"/>
-    <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId17"/>
-    <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId18"/>
-    <sheet name="verifySearchWebinarsHistorical" sheetId="18" r:id="rId19"/>
-    <sheet name="verifyInvalidSearchHistorical" sheetId="19" r:id="rId20"/>
-    <sheet name="verifySortWebinarsHistorical" sheetId="20" r:id="rId21"/>
-    <sheet name="verifyClearSearchHistorical" sheetId="21" r:id="rId22"/>
-    <sheet name="verifyExternalVideo" sheetId="22" r:id="rId23"/>
+    <sheet name="jointUseloginTestAllRoles" sheetId="25" r:id="rId5"/>
+    <sheet name="verifyTheProductLink" sheetId="7" r:id="rId6"/>
+    <sheet name="clickOnOuLink" sheetId="5" r:id="rId7"/>
+    <sheet name="verifyTheSearch" sheetId="6" r:id="rId8"/>
+    <sheet name="verifyTheSearchFullname" sheetId="9" r:id="rId9"/>
+    <sheet name="verifyTheSearchOneAlphabet" sheetId="10" r:id="rId10"/>
+    <sheet name="verifyTheValidationmessage" sheetId="11" r:id="rId11"/>
+    <sheet name="verifyTheSearchfirstname" sheetId="8" r:id="rId12"/>
+    <sheet name="CreateAccountTest" sheetId="4" r:id="rId13"/>
+    <sheet name="verifyTheSearchCrossButton" sheetId="12" r:id="rId14"/>
+    <sheet name="verifyDynamicDropdown" sheetId="13" r:id="rId15"/>
+    <sheet name="verifySearchResultsOnTyping" sheetId="14" r:id="rId16"/>
+    <sheet name="verifyClearButtonOnTyping" sheetId="15" r:id="rId17"/>
+    <sheet name="verifyNoResultsFoundMessage" sheetId="16" r:id="rId18"/>
+    <sheet name="verifySearchTextUpdation" sheetId="17" r:id="rId19"/>
+    <sheet name="verifySearchWebinarsHistorical" sheetId="18" r:id="rId20"/>
+    <sheet name="verifyInvalidSearchHistorical" sheetId="19" r:id="rId21"/>
+    <sheet name="verifySortWebinarsHistorical" sheetId="20" r:id="rId22"/>
+    <sheet name="verifyClearSearchHistorical" sheetId="21" r:id="rId23"/>
+    <sheet name="verifyExternalVideo" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Raman</t>
   </si>
@@ -164,6 +165,12 @@
   </si>
   <si>
     <t>mohammedjunaid.kaikade@centurylink.com</t>
+  </si>
+  <si>
+    <t>ts.allroles@gmail.com</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
   </si>
 </sst>
 </file>
@@ -534,6 +541,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05950B89-E92A-4646-9694-E3FEC191FBC5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10C5F3C-EFE8-4B4F-A0A0-153F52BCD7A9}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -559,7 +589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468D2C47-00AC-4DF8-AF6F-D0EF06E8D38F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -584,7 +614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -612,7 +642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2D0FF7-8259-4C88-ABF2-E9337205FC0D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -637,7 +667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DA5B9-7278-497C-93B8-35FED90EB872}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -662,7 +692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62C1E2F-C94F-40C3-A706-17602DE60785}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -687,7 +717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21843DF4-A28F-40DD-9ED6-86F66E6C735F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -712,7 +742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2497EB80-35A2-4AAD-9C1D-AEDB0EC50212}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -737,7 +767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B1B0C-F841-42B8-A0C1-21DBCE8A2DC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -761,34 +791,6 @@
       </c>
       <c r="B2" t="s">
         <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C461882E-5B05-4789-AF09-7737EACBFC43}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -842,6 +844,34 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C461882E-5B05-4789-AF09-7737EACBFC43}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B5B726-6BA8-4E09-89C1-3903738DA995}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -866,7 +896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C27DB-E6DA-4A1F-9493-A165D018979A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -894,7 +924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE935E1F-C13E-4D89-A48B-2CD047CED7EB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -922,7 +952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A5D42-48F0-4023-83D7-D53E3AC6AFF1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -949,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157B7B6B-70F3-4A49-967B-A759A4B063A2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -985,7 +1015,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,6 +1046,42 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0378AE57-8E4B-4ADE-9C6A-2B26622CCFA6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D1169F-C9EA-4258-B52F-834B03470238}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1060,7 +1126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD1348E-0969-4054-A1EA-4AAF0CCB32EA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1105,7 +1171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E0D8D1-9273-4970-9251-8B99B2980E37}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1133,7 +1199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF90B1B-57B5-4414-AC3B-569DC6A7BEA8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1157,27 +1223,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05950B89-E92A-4646-9694-E3FEC191FBC5}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 18 December 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/com/OSMOSE/excel/testdata.xlsx
+++ b/src/test/resources/com/OSMOSE/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC38373\UI-Automation_New\src\test\resources\com\OSMOSE\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EFCEE2-8DFB-4D80-9BE2-1749E1231699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A88821-4967-4170-BEE7-813D28DB7D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="loginTest" sheetId="1" r:id="rId2"/>
     <sheet name="ocalcloginTestNormal" sheetId="23" r:id="rId3"/>
     <sheet name="ocalcloginTestAdmin" sheetId="24" r:id="rId4"/>
-    <sheet name="jointUseloginTestAllRoles" sheetId="25" r:id="rId5"/>
+    <sheet name="jointUseloginTestSubmitter" sheetId="25" r:id="rId5"/>
     <sheet name="verifyTheProductLink" sheetId="7" r:id="rId6"/>
     <sheet name="clickOnOuLink" sheetId="5" r:id="rId7"/>
     <sheet name="verifyTheSearch" sheetId="6" r:id="rId8"/>
@@ -167,10 +167,10 @@
     <t>mohammedjunaid.kaikade@centurylink.com</t>
   </si>
   <si>
-    <t>ts.allroles@gmail.com</t>
-  </si>
-  <si>
     <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>ts.submitter@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1050,12 +1050,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1068,16 +1068,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:ts.submitter@gmail.com" xr:uid="{2D2CFC26-10A4-4D0A-9261-789EB6A01136}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>